<commit_message>
NHANES QC separate M&F
</commit_message>
<xml_diff>
--- a/docs/eg_data/NHANES/PF/Waist2/BMI/BMI.xlsx
+++ b/docs/eg_data/NHANES/PF/Waist2/BMI/BMI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\NHANES\PF\Waist2\BMI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E122B2F2-D2ED-4556-B77B-821765492615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D79DB6D-A411-4CA5-90D1-21E8BA2B7F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31950" yWindow="-3045" windowWidth="16620" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17145" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NEW(6.28)" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="60">
   <si>
     <t>Plain means</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Family IPR</t>
   </si>
 </sst>
 </file>
@@ -2949,8 +2952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF98E2F-A81A-48C0-B8A9-C127F15DCEAA}">
   <dimension ref="A1:T134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2958,7 +2961,8 @@
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
     <col min="14" max="14" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3081,14 +3085,19 @@
       <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>24</v>
+      <c r="O13" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -3111,16 +3120,23 @@
         <f>B14</f>
         <v>(Intercept)</v>
       </c>
-      <c r="L14" s="2">
-        <f t="shared" ref="L14:M22" si="0">C14</f>
+      <c r="L14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="2">
+        <f>C14</f>
         <v>75713.259375285095</v>
       </c>
-      <c r="M14">
-        <f t="shared" si="0"/>
+      <c r="N14">
+        <f>D14</f>
         <v>1</v>
       </c>
-      <c r="N14" s="16" t="str">
-        <f t="shared" ref="N14:N21" si="1">IF(F14&lt;0.0001,"&lt;0.0001",IF(F14&lt;0.001,"&lt;0.001",IF(F14&lt;0.01,"&lt;0.01",ROUND(F14,3))))</f>
+      <c r="O14" s="2">
+        <f>E14</f>
+        <v>1619.6592675914901</v>
+      </c>
+      <c r="P14" s="16" t="str">
+        <f>IF(F14&lt;0.0001,"&lt;0.0001",IF(F14&lt;0.001,"&lt;0.001",IF(F14&lt;0.01,"&lt;0.01",ROUND(F14,3))))</f>
         <v>&lt;0.0001</v>
       </c>
       <c r="S14" s="1" t="s">
@@ -3147,26 +3163,32 @@
         <v>6.4274207378343497E-3</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" ref="K15:K22" si="2">B15</f>
+        <f t="shared" ref="K15:K22" si="0">B15</f>
         <v>DivGroup</v>
       </c>
-      <c r="L15" s="2">
-        <f t="shared" si="0"/>
+      <c r="L15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" ref="M15:M21" si="1">C15</f>
         <v>575.80939400632599</v>
       </c>
-      <c r="M15">
-        <f t="shared" si="0"/>
+      <c r="N15">
+        <f>D15</f>
         <v>3</v>
       </c>
-      <c r="N15" s="16" t="str">
-        <f t="shared" si="1"/>
+      <c r="O15" s="2">
+        <f>E15</f>
+        <v>4.1059079526433102</v>
+      </c>
+      <c r="P15" s="16" t="str">
+        <f>IF(F15&lt;0.0001,"&lt;0.0001",IF(F15&lt;0.001,"&lt;0.001",IF(F15&lt;0.01,"&lt;0.01",ROUND(F15,3))))</f>
         <v>&lt;0.01</v>
       </c>
       <c r="S15" t="s">
         <v>2</v>
       </c>
       <c r="T15" s="2">
-        <f>C39</f>
         <v>29.233804878220202</v>
       </c>
     </row>
@@ -3187,26 +3209,32 @@
         <v>5.59426293768993E-6</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>age_3</v>
       </c>
-      <c r="L16" s="2">
-        <f t="shared" si="0"/>
+      <c r="L16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="1"/>
         <v>1134.4612065107201</v>
       </c>
-      <c r="M16">
-        <f t="shared" si="0"/>
+      <c r="N16">
+        <f>D16</f>
         <v>2</v>
       </c>
-      <c r="N16" s="16" t="str">
-        <f t="shared" si="1"/>
+      <c r="O16" s="2">
+        <f>E16</f>
+        <v>12.134206227607599</v>
+      </c>
+      <c r="P16" s="16" t="str">
+        <f>IF(F16&lt;0.0001,"&lt;0.0001",IF(F16&lt;0.001,"&lt;0.001",IF(F16&lt;0.01,"&lt;0.01",ROUND(F16,3))))</f>
         <v>&lt;0.0001</v>
       </c>
       <c r="S16" t="s">
         <v>3</v>
       </c>
       <c r="T16" s="2">
-        <f t="shared" ref="T16:T18" si="3">C40</f>
         <v>29.241590661609401</v>
       </c>
     </row>
@@ -3227,26 +3255,32 @@
         <v>2.4300614627646399E-4</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>RIAGENDR</v>
       </c>
-      <c r="L17" s="2">
-        <f t="shared" si="0"/>
+      <c r="L17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="1"/>
         <v>630.71578841036501</v>
       </c>
-      <c r="M17">
-        <f t="shared" si="0"/>
+      <c r="N17">
+        <f>D17</f>
         <v>1</v>
       </c>
-      <c r="N17" s="16" t="str">
-        <f t="shared" si="1"/>
+      <c r="O17" s="2">
+        <f>E17</f>
+        <v>13.492282333952501</v>
+      </c>
+      <c r="P17" s="16" t="str">
+        <f>IF(F17&lt;0.0001,"&lt;0.0001",IF(F17&lt;0.001,"&lt;0.001",IF(F17&lt;0.01,"&lt;0.01",ROUND(F17,3))))</f>
         <v>&lt;0.001</v>
       </c>
       <c r="S17" t="s">
         <v>4</v>
       </c>
       <c r="T17" s="2">
-        <f t="shared" si="3"/>
         <v>29.038371512135399</v>
       </c>
     </row>
@@ -3267,26 +3301,32 @@
         <v>2.72818096336386E-26</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>eth_5</v>
       </c>
-      <c r="L18" s="2">
-        <f t="shared" si="0"/>
+      <c r="L18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="1"/>
         <v>5994.1405933300603</v>
       </c>
-      <c r="M18">
-        <f t="shared" si="0"/>
+      <c r="N18">
+        <f>D18</f>
         <v>4</v>
       </c>
-      <c r="N18" s="16" t="str">
-        <f t="shared" si="1"/>
+      <c r="O18" s="2">
+        <f>E18</f>
+        <v>32.0566880997415</v>
+      </c>
+      <c r="P18" s="16" t="str">
+        <f>IF(F18&lt;0.0001,"&lt;0.0001",IF(F18&lt;0.001,"&lt;0.001",IF(F18&lt;0.01,"&lt;0.01",ROUND(F18,3))))</f>
         <v>&lt;0.0001</v>
       </c>
       <c r="S18" t="s">
         <v>5</v>
       </c>
       <c r="T18" s="2">
-        <f t="shared" si="3"/>
         <v>27.846636199183202</v>
       </c>
     </row>
@@ -3307,19 +3347,26 @@
         <v>0.46195124542618099</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>FIPL</v>
       </c>
-      <c r="L19" s="2">
-        <f t="shared" si="0"/>
+      <c r="L19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="1"/>
         <v>72.219511814502795</v>
       </c>
-      <c r="M19">
-        <f t="shared" si="0"/>
+      <c r="N19">
+        <f>D19</f>
         <v>2</v>
       </c>
-      <c r="N19" s="16">
-        <f t="shared" si="1"/>
+      <c r="O19" s="2">
+        <f>E19</f>
+        <v>0.77246048166746295</v>
+      </c>
+      <c r="P19" s="16">
+        <f>IF(F19&lt;0.0001,"&lt;0.0001",IF(F19&lt;0.001,"&lt;0.001",IF(F19&lt;0.01,"&lt;0.01",ROUND(F19,3))))</f>
         <v>0.46200000000000002</v>
       </c>
     </row>
@@ -3340,19 +3387,26 @@
         <v>3.9835111970400102E-4</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>edu</v>
       </c>
-      <c r="L20" s="2">
-        <f t="shared" si="0"/>
+      <c r="L20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="1"/>
         <v>733.461115876853</v>
       </c>
-      <c r="M20">
-        <f t="shared" si="0"/>
+      <c r="N20">
+        <f>D20</f>
         <v>2</v>
       </c>
-      <c r="N20" s="16" t="str">
-        <f t="shared" si="1"/>
+      <c r="O20" s="2">
+        <f>E20</f>
+        <v>7.8451060194069697</v>
+      </c>
+      <c r="P20" s="16" t="str">
+        <f>IF(F20&lt;0.0001,"&lt;0.0001",IF(F20&lt;0.001,"&lt;0.001",IF(F20&lt;0.01,"&lt;0.01",ROUND(F20,3))))</f>
         <v>&lt;0.001</v>
       </c>
     </row>
@@ -3373,19 +3427,26 @@
         <v>0.20186199649700501</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>KCAL</v>
       </c>
-      <c r="L21" s="2">
-        <f t="shared" si="0"/>
+      <c r="L21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="1"/>
         <v>76.170573350013001</v>
       </c>
-      <c r="M21">
-        <f t="shared" si="0"/>
+      <c r="N21">
+        <f>D21</f>
         <v>1</v>
       </c>
-      <c r="N21" s="16">
-        <f t="shared" si="1"/>
+      <c r="O21" s="2">
+        <f>E21</f>
+        <v>1.6294421355261</v>
+      </c>
+      <c r="P21" s="16">
+        <f>IF(F21&lt;0.0001,"&lt;0.0001",IF(F21&lt;0.001,"&lt;0.001",IF(F21&lt;0.01,"&lt;0.01",ROUND(F21,3))))</f>
         <v>0.20200000000000001</v>
       </c>
     </row>
@@ -3405,18 +3466,23 @@
       <c r="F22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K22" t="str">
-        <f t="shared" si="2"/>
+      <c r="K22" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>Residuals</v>
       </c>
-      <c r="L22" s="2">
-        <f t="shared" si="0"/>
+      <c r="L22" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="M22" s="32">
+        <f>C22</f>
         <v>169455.74339443899</v>
       </c>
-      <c r="M22">
-        <f t="shared" si="0"/>
+      <c r="N22" s="1">
+        <f>D22</f>
         <v>3625</v>
       </c>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -3704,7 +3770,7 @@
         <v>2.5448812352880101</v>
       </c>
       <c r="H32" s="30">
-        <f t="shared" ref="H32:H35" si="4">O32</f>
+        <f t="shared" ref="H32:H35" si="2">O32</f>
         <v>4.2946280616171801E-3</v>
       </c>
       <c r="J32" t="s">
@@ -3750,7 +3816,7 @@
         <v>1.3801541831400499</v>
       </c>
       <c r="H33" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.96245091685531103</v>
       </c>
       <c r="J33" t="s">
@@ -3796,7 +3862,7 @@
         <v>2.5856835278199002</v>
       </c>
       <c r="H34" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>5.57150409061125E-3</v>
       </c>
       <c r="J34" t="s">
@@ -3842,7 +3908,7 @@
         <v>2.6285234816091898</v>
       </c>
       <c r="H35" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>9.1538905871083404E-2</v>
       </c>
       <c r="J35" t="s">
@@ -3909,27 +3975,27 @@
         <v>DivNA</v>
       </c>
       <c r="B39" t="str">
-        <f t="shared" ref="B39:G39" si="5">B26</f>
+        <f t="shared" ref="B39:G39" si="3">B26</f>
         <v>.</v>
       </c>
       <c r="C39" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>29.233804878220202</v>
       </c>
       <c r="D39" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0.20968120301689799</v>
       </c>
       <c r="E39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>3625</v>
       </c>
       <c r="F39" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>28.644862022538302</v>
       </c>
       <c r="G39" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>29.822747733902101</v>
       </c>
       <c r="H39" t="s">
@@ -3938,31 +4004,31 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f t="shared" ref="A40:G48" si="6">A27</f>
+        <f t="shared" ref="A40:G48" si="4">A27</f>
         <v>Div0</v>
       </c>
       <c r="B40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="C40" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>29.241590661609401</v>
       </c>
       <c r="D40" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.24374289869233201</v>
       </c>
       <c r="E40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F40" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>28.556976892026601</v>
       </c>
       <c r="G40" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>29.9262044311922</v>
       </c>
       <c r="H40" t="s">
@@ -3971,31 +4037,31 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>Div1</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="C41" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>29.038371512135399</v>
       </c>
       <c r="D41" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.38453660956396801</v>
       </c>
       <c r="E41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F41" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>27.9583028856091</v>
       </c>
       <c r="G41" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>30.1184401386618</v>
       </c>
       <c r="H41" t="s">
@@ -4004,31 +4070,31 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>Div2</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="C42" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>27.846636199183202</v>
       </c>
       <c r="D42" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.39079291078135497</v>
       </c>
       <c r="E42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F42" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>26.748995163437701</v>
       </c>
       <c r="G42" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>28.944277234928698</v>
       </c>
       <c r="H42" t="s">
@@ -4037,31 +4103,31 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="B43" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>DivNA - Div0</v>
       </c>
       <c r="C43" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-7.78578338916802E-3</v>
       </c>
       <c r="D43" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.26435514357971601</v>
       </c>
       <c r="E43" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F43" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-0.75029427215198097</v>
       </c>
       <c r="G43" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.73472270537364504</v>
       </c>
       <c r="H43" s="17">
@@ -4071,171 +4137,171 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>DivNA - Div1</v>
       </c>
       <c r="C44" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.19543336608478501</v>
       </c>
       <c r="D44" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.40463655535146398</v>
       </c>
       <c r="E44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F44" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-0.941091057627087</v>
       </c>
       <c r="G44" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.3319577897966599</v>
       </c>
       <c r="H44" s="16">
-        <f t="shared" ref="H44:H48" si="7">IF(H31&lt;0.0001,"&lt;0.0001",IF(H31&lt;0.001,"&lt;0.001",IF(H31&lt;0.01,"&lt;0.01",ROUND(H31,3))))</f>
+        <f t="shared" ref="H44:H48" si="5">IF(H31&lt;0.0001,"&lt;0.0001",IF(H31&lt;0.001,"&lt;0.001",IF(H31&lt;0.01,"&lt;0.01",ROUND(H31,3))))</f>
         <v>0.96299999999999997</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>DivNA - Div2</v>
       </c>
       <c r="C45" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.3871686790370099</v>
       </c>
       <c r="D45" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.41218016179412997</v>
       </c>
       <c r="E45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F45" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.22945612278602101</v>
       </c>
       <c r="G45" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.5448812352880101</v>
       </c>
       <c r="H45" s="16" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>&lt;0.01</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="B46" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>Div0 - Div1</v>
       </c>
       <c r="C46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.203219149473953</v>
       </c>
       <c r="D46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.419023936449816</v>
       </c>
       <c r="E46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-0.97371588419213895</v>
       </c>
       <c r="G46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.3801541831400499</v>
       </c>
       <c r="H46" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0.96199999999999997</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="B47" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>Div0 - Div2</v>
       </c>
       <c r="C47" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.39495446242618</v>
       </c>
       <c r="D47" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.423935022710899</v>
       </c>
       <c r="E47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F47" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.20422539703246001</v>
       </c>
       <c r="G47" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.5856835278199002</v>
       </c>
       <c r="H47" s="16" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>&lt;0.01</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>.</v>
       </c>
       <c r="B48" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>Div1 - Div2</v>
       </c>
       <c r="C48" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.1917353129522299</v>
       </c>
       <c r="D48" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.51153939431967799</v>
       </c>
       <c r="E48" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>3625</v>
       </c>
       <c r="F48" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>-0.24505285570473401</v>
       </c>
       <c r="G48" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.6285234816091898</v>
       </c>
       <c r="H48" s="18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
@@ -4305,26 +4371,26 @@
         <v>0</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" ref="J55:J61" si="8">B55</f>
+        <f t="shared" ref="J55:J61" si="6">B55</f>
         <v>(Intercept)</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L55" s="2">
-        <f t="shared" ref="L55:M61" si="9">C55</f>
+        <f t="shared" ref="L55:M61" si="7">C55</f>
         <v>161079.753365293</v>
       </c>
       <c r="M55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="N55" s="2">
-        <f>E55</f>
+        <f t="shared" ref="N55:N60" si="8">E55</f>
         <v>3445.7599769502699</v>
       </c>
       <c r="O55" s="16" t="str">
-        <f>IF(F55&lt;0.0001,"&lt;0.0001",IF(F55&lt;0.001,"&lt;0.001",IF(F55&lt;0.01,"&lt;0.01",ROUND(F55,3))))</f>
+        <f t="shared" ref="O55:O60" si="9">IF(F55&lt;0.0001,"&lt;0.0001",IF(F55&lt;0.001,"&lt;0.001",IF(F55&lt;0.01,"&lt;0.01",ROUND(F55,3))))</f>
         <v>&lt;0.0001</v>
       </c>
     </row>
@@ -4345,26 +4411,26 @@
         <v>8.2062289630025296E-3</v>
       </c>
       <c r="J56" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>DivGroup</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>1</v>
       </c>
       <c r="L56" s="2">
+        <f t="shared" si="7"/>
+        <v>551.12872435804502</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="N56" s="2">
+        <f t="shared" si="8"/>
+        <v>3.92984895342282</v>
+      </c>
+      <c r="O56" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>551.12872435804502</v>
-      </c>
-      <c r="M56">
-        <f t="shared" si="9"/>
-        <v>3</v>
-      </c>
-      <c r="N56" s="2">
-        <f>E56</f>
-        <v>3.92984895342282</v>
-      </c>
-      <c r="O56" s="16" t="str">
-        <f>IF(F56&lt;0.0001,"&lt;0.0001",IF(F56&lt;0.001,"&lt;0.001",IF(F56&lt;0.01,"&lt;0.01",ROUND(F56,3))))</f>
         <v>&lt;0.01</v>
       </c>
     </row>
@@ -4385,26 +4451,26 @@
         <v>9.2947095523864707E-6</v>
       </c>
       <c r="J57" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>age_3</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>51</v>
       </c>
       <c r="L57" s="2">
+        <f t="shared" si="7"/>
+        <v>1086.69973258706</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="N57" s="2">
+        <f t="shared" si="8"/>
+        <v>11.623144334655599</v>
+      </c>
+      <c r="O57" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>1086.69973258706</v>
-      </c>
-      <c r="M57">
-        <f t="shared" si="9"/>
-        <v>2</v>
-      </c>
-      <c r="N57" s="2">
-        <f>E57</f>
-        <v>11.623144334655599</v>
-      </c>
-      <c r="O57" s="16" t="str">
-        <f>IF(F57&lt;0.0001,"&lt;0.0001",IF(F57&lt;0.001,"&lt;0.001",IF(F57&lt;0.01,"&lt;0.01",ROUND(F57,3))))</f>
         <v>&lt;0.0001</v>
       </c>
     </row>
@@ -4425,26 +4491,26 @@
         <v>5.3179708572879795E-4</v>
       </c>
       <c r="J58" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>RIAGENDR</v>
       </c>
       <c r="K58" s="2" t="s">
         <v>52</v>
       </c>
       <c r="L58" s="2">
+        <f t="shared" si="7"/>
+        <v>562.00738546336697</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N58" s="2">
+        <f t="shared" si="8"/>
+        <v>12.0222592543241</v>
+      </c>
+      <c r="O58" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>562.00738546336697</v>
-      </c>
-      <c r="M58">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="N58" s="2">
-        <f>E58</f>
-        <v>12.0222592543241</v>
-      </c>
-      <c r="O58" s="16" t="str">
-        <f>IF(F58&lt;0.0001,"&lt;0.0001",IF(F58&lt;0.001,"&lt;0.001",IF(F58&lt;0.01,"&lt;0.01",ROUND(F58,3))))</f>
         <v>&lt;0.001</v>
       </c>
     </row>
@@ -4465,26 +4531,26 @@
         <v>1.6934425061199598E-27</v>
       </c>
       <c r="J59" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>eth_5</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>53</v>
       </c>
       <c r="L59" s="2">
+        <f t="shared" si="7"/>
+        <v>6267.5231195289198</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="N59" s="2">
+        <f t="shared" si="8"/>
+        <v>33.518148415132501</v>
+      </c>
+      <c r="O59" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>6267.5231195289198</v>
-      </c>
-      <c r="M59">
-        <f t="shared" si="9"/>
-        <v>4</v>
-      </c>
-      <c r="N59" s="2">
-        <f>E59</f>
-        <v>33.518148415132501</v>
-      </c>
-      <c r="O59" s="16" t="str">
-        <f>IF(F59&lt;0.0001,"&lt;0.0001",IF(F59&lt;0.001,"&lt;0.001",IF(F59&lt;0.01,"&lt;0.01",ROUND(F59,3))))</f>
         <v>&lt;0.0001</v>
       </c>
     </row>
@@ -4505,26 +4571,26 @@
         <v>1.22230982793797E-4</v>
       </c>
       <c r="J60" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>edu</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>54</v>
       </c>
       <c r="L60" s="2">
+        <f t="shared" si="7"/>
+        <v>844.44291276141303</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="N60" s="2">
+        <f t="shared" si="8"/>
+        <v>9.03200908500874</v>
+      </c>
+      <c r="O60" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>844.44291276141303</v>
-      </c>
-      <c r="M60">
-        <f t="shared" si="9"/>
-        <v>2</v>
-      </c>
-      <c r="N60" s="2">
-        <f>E60</f>
-        <v>9.03200908500874</v>
-      </c>
-      <c r="O60" s="16" t="str">
-        <f>IF(F60&lt;0.0001,"&lt;0.0001",IF(F60&lt;0.001,"&lt;0.001",IF(F60&lt;0.01,"&lt;0.01",ROUND(F60,3))))</f>
         <v>&lt;0.001</v>
       </c>
     </row>
@@ -4545,18 +4611,18 @@
         <v>27</v>
       </c>
       <c r="J61" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>Residuals</v>
       </c>
       <c r="K61" s="32" t="s">
         <v>26</v>
       </c>
       <c r="L61" s="32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>169598.97065335201</v>
       </c>
       <c r="M61" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>3628</v>
       </c>
       <c r="N61" s="33"/>

</xml_diff>